<commit_message>
ajout document de conception + notes
</commit_message>
<xml_diff>
--- a/C61/Sprint0/doc/Maquettes.xlsx
+++ b/C61/Sprint0/doc/Maquettes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\travail\Projet Synthese\C61_Projet_synthese\C61\Sprint0\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DEEC68-C2B8-4B8B-AB2C-9328159C5D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D244E1D-386D-4C76-B8EA-6995F75B1BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9981ABF-3526-4808-BFAB-E37EF0B37502}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="127">
-  <si>
-    <t>Crypto-Nooby</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="122">
   <si>
     <t>Créer un compte</t>
   </si>
@@ -378,24 +375,9 @@
     <t>Exemple de mofication du mot de passe :</t>
   </si>
   <si>
-    <t>Exemple de modification du type de profil :</t>
-  </si>
-  <si>
-    <t>Changer son type de compte</t>
-  </si>
-  <si>
-    <t>Poule</t>
-  </si>
-  <si>
-    <t>Montant dans le compte :</t>
-  </si>
-  <si>
     <t>Nouveau type de ocmpte :</t>
   </si>
   <si>
-    <t>Type de compte actuel :</t>
-  </si>
-  <si>
     <t>Exemple de modification du courriel :</t>
   </si>
   <si>
@@ -415,6 +397,9 @@
   </si>
   <si>
     <t>Page d'accueil avant la connexion</t>
+  </si>
+  <si>
+    <t>Crypto Newbie</t>
   </si>
 </sst>
 </file>
@@ -748,7 +733,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -870,24 +855,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="6" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -896,22 +870,34 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="6" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -920,13 +906,13 @@
     <xf numFmtId="6" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2077,10 +2063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86EF0CA-617E-4DFF-A0C4-6660ED4E21B6}">
-  <dimension ref="B1:AA296"/>
+  <dimension ref="B1:AA284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="A253" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E263" sqref="E263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2092,46 +2078,46 @@
   <sheetData>
     <row r="1" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="2:21" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="105" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
+        <v>11</v>
+      </c>
+      <c r="E3" s="103" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
       <c r="H3" s="6"/>
       <c r="I3" s="5"/>
       <c r="J3" s="7"/>
-      <c r="M3" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3" s="102"/>
+      <c r="M3" s="97" t="s">
+        <v>121</v>
+      </c>
+      <c r="N3" s="97"/>
       <c r="O3" s="33"/>
       <c r="P3" s="30"/>
       <c r="Q3" s="30"/>
       <c r="R3" s="30"/>
       <c r="S3" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="T3" s="112" t="s">
-        <v>1</v>
-      </c>
-      <c r="U3" s="113"/>
+        <v>3</v>
+      </c>
+      <c r="T3" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="U3" s="102"/>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B4" s="8"/>
@@ -2157,18 +2143,18 @@
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
+      <c r="E5" s="104"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="104"/>
       <c r="H5" s="10"/>
       <c r="I5" s="9"/>
       <c r="J5" s="11"/>
       <c r="M5" s="22"/>
       <c r="N5" s="34"/>
       <c r="O5" s="23"/>
-      <c r="P5" s="99"/>
-      <c r="Q5" s="99"/>
-      <c r="R5" s="99"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="95"/>
+      <c r="R5" s="95"/>
       <c r="S5" s="23"/>
       <c r="T5" s="23"/>
       <c r="U5" s="24"/>
@@ -2197,11 +2183,11 @@
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="111" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="111"/>
-      <c r="G7" s="111"/>
+      <c r="E7" s="105" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="105"/>
+      <c r="G7" s="105"/>
       <c r="H7" s="10"/>
       <c r="I7" s="9"/>
       <c r="J7" s="11"/>
@@ -2251,19 +2237,19 @@
       <c r="P9" s="10"/>
       <c r="Q9" s="19"/>
       <c r="R9" s="19"/>
-      <c r="S9" s="106" t="s">
-        <v>22</v>
-      </c>
-      <c r="T9" s="107"/>
+      <c r="S9" s="98" t="s">
+        <v>21</v>
+      </c>
+      <c r="T9" s="99"/>
       <c r="U9" s="27"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B10" s="8"/>
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="104"/>
-      <c r="F10" s="104"/>
-      <c r="G10" s="104"/>
+      <c r="E10" s="100"/>
+      <c r="F10" s="100"/>
+      <c r="G10" s="100"/>
       <c r="H10" s="10"/>
       <c r="I10" s="9"/>
       <c r="J10" s="11"/>
@@ -2288,15 +2274,15 @@
       <c r="I11" s="9"/>
       <c r="J11" s="11"/>
       <c r="M11" s="26"/>
-      <c r="N11" s="104" t="s">
-        <v>23</v>
-      </c>
-      <c r="O11" s="104"/>
-      <c r="P11" s="104"/>
-      <c r="Q11" s="104"/>
-      <c r="R11" s="104"/>
-      <c r="S11" s="104"/>
-      <c r="T11" s="104"/>
+      <c r="N11" s="100" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" s="100"/>
+      <c r="P11" s="100"/>
+      <c r="Q11" s="100"/>
+      <c r="R11" s="100"/>
+      <c r="S11" s="100"/>
+      <c r="T11" s="100"/>
       <c r="U11" s="27"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.3">
@@ -2304,7 +2290,7 @@
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="3"/>
@@ -2312,15 +2298,15 @@
       <c r="I12" s="9"/>
       <c r="J12" s="11"/>
       <c r="M12" s="26"/>
-      <c r="N12" s="104" t="s">
-        <v>24</v>
-      </c>
-      <c r="O12" s="104"/>
-      <c r="P12" s="104"/>
-      <c r="Q12" s="104"/>
-      <c r="R12" s="104"/>
-      <c r="S12" s="104"/>
-      <c r="T12" s="104"/>
+      <c r="N12" s="100" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" s="100"/>
+      <c r="P12" s="100"/>
+      <c r="Q12" s="100"/>
+      <c r="R12" s="100"/>
+      <c r="S12" s="100"/>
+      <c r="T12" s="100"/>
       <c r="U12" s="27"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.3">
@@ -2334,15 +2320,15 @@
       <c r="I13" s="9"/>
       <c r="J13" s="11"/>
       <c r="M13" s="26"/>
-      <c r="N13" s="104" t="s">
-        <v>25</v>
-      </c>
-      <c r="O13" s="104"/>
-      <c r="P13" s="104"/>
-      <c r="Q13" s="104"/>
-      <c r="R13" s="104"/>
-      <c r="S13" s="104"/>
-      <c r="T13" s="104"/>
+      <c r="N13" s="100" t="s">
+        <v>24</v>
+      </c>
+      <c r="O13" s="100"/>
+      <c r="P13" s="100"/>
+      <c r="Q13" s="100"/>
+      <c r="R13" s="100"/>
+      <c r="S13" s="100"/>
+      <c r="T13" s="100"/>
       <c r="U13" s="27"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.3">
@@ -2350,7 +2336,7 @@
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="3"/>
@@ -2358,15 +2344,15 @@
       <c r="I14" s="9"/>
       <c r="J14" s="11"/>
       <c r="M14" s="26"/>
-      <c r="N14" s="104" t="s">
-        <v>26</v>
-      </c>
-      <c r="O14" s="104"/>
-      <c r="P14" s="104"/>
-      <c r="Q14" s="104"/>
-      <c r="R14" s="104"/>
-      <c r="S14" s="104"/>
-      <c r="T14" s="104"/>
+      <c r="N14" s="100" t="s">
+        <v>25</v>
+      </c>
+      <c r="O14" s="100"/>
+      <c r="P14" s="100"/>
+      <c r="Q14" s="100"/>
+      <c r="R14" s="100"/>
+      <c r="S14" s="100"/>
+      <c r="T14" s="100"/>
       <c r="U14" s="27"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.3">
@@ -2380,39 +2366,39 @@
       <c r="I15" s="9"/>
       <c r="J15" s="11"/>
       <c r="M15" s="26"/>
-      <c r="N15" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="O15" s="104"/>
-      <c r="P15" s="104"/>
-      <c r="Q15" s="104"/>
-      <c r="R15" s="104"/>
-      <c r="S15" s="104"/>
-      <c r="T15" s="104"/>
+      <c r="N15" s="100" t="s">
+        <v>26</v>
+      </c>
+      <c r="O15" s="100"/>
+      <c r="P15" s="100"/>
+      <c r="Q15" s="100"/>
+      <c r="R15" s="100"/>
+      <c r="S15" s="100"/>
+      <c r="T15" s="100"/>
       <c r="U15" s="27"/>
     </row>
     <row r="16" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="108" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="99"/>
-      <c r="G16" s="99"/>
+      <c r="E16" s="106" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="95"/>
+      <c r="G16" s="95"/>
       <c r="H16" s="10"/>
       <c r="I16" s="9"/>
       <c r="J16" s="11"/>
       <c r="M16" s="26"/>
-      <c r="N16" s="104" t="s">
-        <v>28</v>
-      </c>
-      <c r="O16" s="104"/>
-      <c r="P16" s="104"/>
-      <c r="Q16" s="104"/>
-      <c r="R16" s="104"/>
-      <c r="S16" s="104"/>
-      <c r="T16" s="104"/>
+      <c r="N16" s="100" t="s">
+        <v>27</v>
+      </c>
+      <c r="O16" s="100"/>
+      <c r="P16" s="100"/>
+      <c r="Q16" s="100"/>
+      <c r="R16" s="100"/>
+      <c r="S16" s="100"/>
+      <c r="T16" s="100"/>
       <c r="U16" s="27"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.3">
@@ -2426,15 +2412,15 @@
       <c r="I17" s="9"/>
       <c r="J17" s="11"/>
       <c r="M17" s="26"/>
-      <c r="N17" s="104" t="s">
-        <v>29</v>
-      </c>
-      <c r="O17" s="104"/>
-      <c r="P17" s="104"/>
-      <c r="Q17" s="104"/>
-      <c r="R17" s="104"/>
-      <c r="S17" s="104"/>
-      <c r="T17" s="104"/>
+      <c r="N17" s="100" t="s">
+        <v>28</v>
+      </c>
+      <c r="O17" s="100"/>
+      <c r="P17" s="100"/>
+      <c r="Q17" s="100"/>
+      <c r="R17" s="100"/>
+      <c r="S17" s="100"/>
+      <c r="T17" s="100"/>
       <c r="U17" s="27"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.3">
@@ -2490,20 +2476,20 @@
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="2:21" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="105" t="s">
-        <v>0</v>
-      </c>
-      <c r="F24" s="105"/>
-      <c r="G24" s="105"/>
+        <v>11</v>
+      </c>
+      <c r="E24" s="103" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" s="103"/>
+      <c r="G24" s="103"/>
       <c r="H24" s="6"/>
       <c r="I24" s="5"/>
       <c r="J24" s="7"/>
@@ -2523,11 +2509,11 @@
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="97" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="97"/>
-      <c r="G26" s="97"/>
+      <c r="E26" s="104" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="104"/>
+      <c r="G26" s="104"/>
       <c r="H26" s="10"/>
       <c r="I26" s="9"/>
       <c r="J26" s="11"/>
@@ -2548,7 +2534,7 @@
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
       <c r="E28" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="21"/>
@@ -2572,7 +2558,7 @@
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
@@ -2596,7 +2582,7 @@
       <c r="C32" s="9"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" s="20"/>
       <c r="G32" s="21"/>
@@ -2620,7 +2606,7 @@
       <c r="C34" s="9"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" s="20"/>
       <c r="G34" s="21"/>
@@ -2644,7 +2630,7 @@
       <c r="C36" s="9"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F36" s="20"/>
       <c r="G36" s="21"/>
@@ -2668,7 +2654,7 @@
       <c r="C38" s="9"/>
       <c r="D38" s="10"/>
       <c r="E38" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F38" s="20"/>
       <c r="G38" s="21"/>
@@ -2691,17 +2677,17 @@
       <c r="B40" s="8"/>
       <c r="C40" s="9"/>
       <c r="D40" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E40" s="17"/>
       <c r="F40" s="86" t="s">
+        <v>96</v>
+      </c>
+      <c r="G40" s="88" t="s">
         <v>97</v>
       </c>
-      <c r="G40" s="88" t="s">
+      <c r="H40" s="87" t="s">
         <v>98</v>
-      </c>
-      <c r="H40" s="87" t="s">
-        <v>99</v>
       </c>
       <c r="I40" s="9"/>
       <c r="J40" s="11"/>
@@ -2721,11 +2707,11 @@
       <c r="B42" s="8"/>
       <c r="C42" s="9"/>
       <c r="D42" s="10"/>
-      <c r="E42" s="98" t="s">
-        <v>100</v>
-      </c>
-      <c r="F42" s="98"/>
-      <c r="G42" s="98"/>
+      <c r="E42" s="111" t="s">
+        <v>99</v>
+      </c>
+      <c r="F42" s="111"/>
+      <c r="G42" s="111"/>
       <c r="H42" s="10"/>
       <c r="I42" s="9"/>
       <c r="J42" s="11"/>
@@ -2743,34 +2729,34 @@
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B46" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B47" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="102"/>
+      <c r="B47" s="97" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" s="97"/>
       <c r="D47" s="33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E47" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F47" s="30" t="s">
+      <c r="G47" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="G47" s="30" t="s">
+      <c r="H47" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="H47" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="I47" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J47" s="32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.3">
@@ -2787,12 +2773,12 @@
     <row r="49" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B49" s="22"/>
       <c r="C49" s="34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D49" s="23"/>
-      <c r="E49" s="99"/>
-      <c r="F49" s="99"/>
-      <c r="G49" s="99"/>
+      <c r="E49" s="95"/>
+      <c r="F49" s="95"/>
+      <c r="G49" s="95"/>
       <c r="H49" s="23"/>
       <c r="I49" s="23"/>
       <c r="J49" s="24"/>
@@ -2833,18 +2819,18 @@
     <row r="53" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B53" s="26"/>
       <c r="C53" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G53" s="19"/>
-      <c r="H53" s="106" t="s">
-        <v>22</v>
-      </c>
-      <c r="I53" s="107"/>
+      <c r="H53" s="98" t="s">
+        <v>21</v>
+      </c>
+      <c r="I53" s="99"/>
       <c r="J53" s="27"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.3">
@@ -2860,93 +2846,93 @@
     </row>
     <row r="55" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="26"/>
-      <c r="C55" s="104" t="s">
-        <v>23</v>
-      </c>
-      <c r="D55" s="104"/>
-      <c r="E55" s="104"/>
-      <c r="F55" s="104"/>
-      <c r="G55" s="104"/>
-      <c r="H55" s="104"/>
-      <c r="I55" s="104"/>
+      <c r="C55" s="100" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="100"/>
+      <c r="E55" s="100"/>
+      <c r="F55" s="100"/>
+      <c r="G55" s="100"/>
+      <c r="H55" s="100"/>
+      <c r="I55" s="100"/>
       <c r="J55" s="27"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B56" s="26"/>
-      <c r="C56" s="104" t="s">
-        <v>24</v>
-      </c>
-      <c r="D56" s="104"/>
-      <c r="E56" s="104"/>
-      <c r="F56" s="104"/>
-      <c r="G56" s="104"/>
-      <c r="H56" s="104"/>
-      <c r="I56" s="104"/>
+      <c r="C56" s="100" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" s="100"/>
+      <c r="E56" s="100"/>
+      <c r="F56" s="100"/>
+      <c r="G56" s="100"/>
+      <c r="H56" s="100"/>
+      <c r="I56" s="100"/>
       <c r="J56" s="27"/>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B57" s="26"/>
-      <c r="C57" s="104" t="s">
-        <v>25</v>
-      </c>
-      <c r="D57" s="104"/>
-      <c r="E57" s="104"/>
-      <c r="F57" s="104"/>
-      <c r="G57" s="104"/>
-      <c r="H57" s="104"/>
-      <c r="I57" s="104"/>
+      <c r="C57" s="100" t="s">
+        <v>24</v>
+      </c>
+      <c r="D57" s="100"/>
+      <c r="E57" s="100"/>
+      <c r="F57" s="100"/>
+      <c r="G57" s="100"/>
+      <c r="H57" s="100"/>
+      <c r="I57" s="100"/>
       <c r="J57" s="27"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B58" s="26"/>
-      <c r="C58" s="104" t="s">
-        <v>26</v>
-      </c>
-      <c r="D58" s="104"/>
-      <c r="E58" s="104"/>
-      <c r="F58" s="104"/>
-      <c r="G58" s="104"/>
-      <c r="H58" s="104"/>
-      <c r="I58" s="104"/>
+      <c r="C58" s="100" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58" s="100"/>
+      <c r="E58" s="100"/>
+      <c r="F58" s="100"/>
+      <c r="G58" s="100"/>
+      <c r="H58" s="100"/>
+      <c r="I58" s="100"/>
       <c r="J58" s="27"/>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B59" s="26"/>
-      <c r="C59" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="D59" s="104"/>
-      <c r="E59" s="104"/>
-      <c r="F59" s="104"/>
-      <c r="G59" s="104"/>
-      <c r="H59" s="104"/>
-      <c r="I59" s="104"/>
+      <c r="C59" s="100" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="100"/>
+      <c r="E59" s="100"/>
+      <c r="F59" s="100"/>
+      <c r="G59" s="100"/>
+      <c r="H59" s="100"/>
+      <c r="I59" s="100"/>
       <c r="J59" s="27"/>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B60" s="26"/>
-      <c r="C60" s="104" t="s">
-        <v>28</v>
-      </c>
-      <c r="D60" s="104"/>
-      <c r="E60" s="104"/>
-      <c r="F60" s="104"/>
-      <c r="G60" s="104"/>
-      <c r="H60" s="104"/>
-      <c r="I60" s="104"/>
+      <c r="C60" s="100" t="s">
+        <v>27</v>
+      </c>
+      <c r="D60" s="100"/>
+      <c r="E60" s="100"/>
+      <c r="F60" s="100"/>
+      <c r="G60" s="100"/>
+      <c r="H60" s="100"/>
+      <c r="I60" s="100"/>
       <c r="J60" s="27"/>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B61" s="26"/>
-      <c r="C61" s="104" t="s">
-        <v>29</v>
-      </c>
-      <c r="D61" s="104"/>
-      <c r="E61" s="104"/>
-      <c r="F61" s="104"/>
-      <c r="G61" s="104"/>
-      <c r="H61" s="104"/>
-      <c r="I61" s="104"/>
+      <c r="C61" s="100" t="s">
+        <v>28</v>
+      </c>
+      <c r="D61" s="100"/>
+      <c r="E61" s="100"/>
+      <c r="F61" s="100"/>
+      <c r="G61" s="100"/>
+      <c r="H61" s="100"/>
+      <c r="I61" s="100"/>
       <c r="J61" s="27"/>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.3">
@@ -2963,7 +2949,7 @@
     <row r="63" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B63" s="26"/>
       <c r="C63" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D63" s="17"/>
       <c r="E63" s="17"/>
@@ -2986,34 +2972,34 @@
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B68" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="69" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B69" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="C69" s="102"/>
+      <c r="B69" s="97" t="s">
+        <v>121</v>
+      </c>
+      <c r="C69" s="97"/>
       <c r="D69" s="33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E69" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F69" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F69" s="30" t="s">
+      <c r="G69" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="G69" s="30" t="s">
+      <c r="H69" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="H69" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="I69" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J69" s="32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.3">
@@ -3030,12 +3016,12 @@
     <row r="71" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B71" s="22"/>
       <c r="C71" s="34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D71" s="23"/>
-      <c r="E71" s="99"/>
-      <c r="F71" s="99"/>
-      <c r="G71" s="99"/>
+      <c r="E71" s="95"/>
+      <c r="F71" s="95"/>
+      <c r="G71" s="95"/>
       <c r="H71" s="23"/>
       <c r="I71" s="23"/>
       <c r="J71" s="24"/>
@@ -3076,7 +3062,7 @@
     <row r="75" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B75" s="26"/>
       <c r="C75" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D75" s="10"/>
       <c r="E75" s="10"/>
@@ -3084,7 +3070,7 @@
       <c r="G75" s="19"/>
       <c r="H75" s="17"/>
       <c r="I75" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J75" s="27"/>
     </row>
@@ -3102,7 +3088,7 @@
     <row r="77" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B77" s="26"/>
       <c r="C77" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D77" s="17"/>
       <c r="E77" s="17"/>
@@ -3170,7 +3156,7 @@
     <row r="83" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B83" s="26"/>
       <c r="C83" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D83" s="17"/>
       <c r="E83" s="17"/>
@@ -3183,38 +3169,38 @@
     <row r="84" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B84" s="26"/>
       <c r="C84" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D84" s="37"/>
       <c r="E84" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F84" s="37"/>
       <c r="G84" s="37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H84" s="37"/>
       <c r="I84" s="38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J84" s="27"/>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B85" s="26"/>
       <c r="C85" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D85" s="42"/>
       <c r="E85" s="42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F85" s="42"/>
       <c r="G85" s="42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H85" s="42"/>
       <c r="I85" s="43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J85" s="27"/>
     </row>
@@ -3231,34 +3217,34 @@
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B91" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="92" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B92" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="C92" s="102"/>
+      <c r="B92" s="97" t="s">
+        <v>121</v>
+      </c>
+      <c r="C92" s="97"/>
       <c r="D92" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E92" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="F92" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F92" s="30" t="s">
+      <c r="G92" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="G92" s="30" t="s">
+      <c r="H92" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="H92" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="I92" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J92" s="32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.3">
@@ -3275,12 +3261,12 @@
     <row r="94" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B94" s="22"/>
       <c r="C94" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D94" s="23"/>
-      <c r="E94" s="99"/>
-      <c r="F94" s="99"/>
-      <c r="G94" s="99"/>
+      <c r="E94" s="95"/>
+      <c r="F94" s="95"/>
+      <c r="G94" s="95"/>
       <c r="H94" s="23"/>
       <c r="I94" s="23"/>
       <c r="J94" s="24"/>
@@ -3300,11 +3286,11 @@
       <c r="B96" s="26"/>
       <c r="C96" s="10"/>
       <c r="D96" s="10"/>
-      <c r="E96" s="101" t="s">
-        <v>42</v>
-      </c>
-      <c r="F96" s="101"/>
-      <c r="G96" s="101"/>
+      <c r="E96" s="96" t="s">
+        <v>41</v>
+      </c>
+      <c r="F96" s="96"/>
+      <c r="G96" s="96"/>
       <c r="H96" s="10"/>
       <c r="I96" s="10"/>
       <c r="J96" s="27"/>
@@ -3313,11 +3299,11 @@
       <c r="B97" s="26"/>
       <c r="C97" s="10"/>
       <c r="D97" s="10"/>
-      <c r="E97" s="103">
+      <c r="E97" s="107">
         <v>5000</v>
       </c>
-      <c r="F97" s="103"/>
-      <c r="G97" s="103"/>
+      <c r="F97" s="107"/>
+      <c r="G97" s="107"/>
       <c r="H97" s="10"/>
       <c r="I97" s="10"/>
       <c r="J97" s="27"/>
@@ -3333,17 +3319,17 @@
     <row r="99" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B99" s="26"/>
       <c r="C99" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D99" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D99" s="10" t="s">
+      <c r="E99" s="17" t="s">
         <v>45</v>
-      </c>
-      <c r="E99" s="17" t="s">
-        <v>46</v>
       </c>
       <c r="F99" s="17"/>
       <c r="G99" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H99" s="10"/>
       <c r="I99" s="10"/>
@@ -3352,63 +3338,63 @@
     <row r="100" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B100" s="26"/>
       <c r="C100" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D100" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E100" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F100" s="17"/>
       <c r="G100" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H100" s="17"/>
       <c r="I100" s="48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J100" s="27"/>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B101" s="26"/>
       <c r="C101" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D101" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E101" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F101" s="17"/>
       <c r="G101" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H101" s="17"/>
       <c r="I101" s="48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J101" s="27"/>
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B102" s="26"/>
       <c r="C102" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D102" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E102" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F102" s="17"/>
       <c r="G102" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H102" s="17"/>
       <c r="I102" s="48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J102" s="27"/>
     </row>
@@ -3418,7 +3404,7 @@
       <c r="D103" s="17"/>
       <c r="E103" s="17"/>
       <c r="F103" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G103" s="17"/>
       <c r="H103" s="17"/>
@@ -3492,30 +3478,30 @@
       <c r="J109" s="29"/>
     </row>
     <row r="111" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B111" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="C111" s="102"/>
+      <c r="B111" s="97" t="s">
+        <v>121</v>
+      </c>
+      <c r="C111" s="97"/>
       <c r="D111" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E111" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="F111" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F111" s="30" t="s">
+      <c r="G111" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="G111" s="30" t="s">
+      <c r="H111" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="H111" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="I111" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J111" s="32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="112" spans="2:10" x14ac:dyDescent="0.3">
@@ -3532,12 +3518,12 @@
     <row r="113" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B113" s="22"/>
       <c r="C113" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D113" s="23"/>
-      <c r="E113" s="99"/>
-      <c r="F113" s="99"/>
-      <c r="G113" s="99"/>
+      <c r="E113" s="95"/>
+      <c r="F113" s="95"/>
+      <c r="G113" s="95"/>
       <c r="H113" s="23"/>
       <c r="I113" s="23"/>
       <c r="J113" s="24"/>
@@ -3557,9 +3543,9 @@
       <c r="B115" s="49"/>
       <c r="C115" s="50"/>
       <c r="D115" s="50"/>
-      <c r="E115" s="109"/>
-      <c r="F115" s="109"/>
-      <c r="G115" s="109"/>
+      <c r="E115" s="108"/>
+      <c r="F115" s="108"/>
+      <c r="G115" s="108"/>
       <c r="H115" s="50"/>
       <c r="I115" s="50"/>
       <c r="J115" s="51"/>
@@ -3568,9 +3554,9 @@
       <c r="B116" s="49"/>
       <c r="C116" s="50"/>
       <c r="D116" s="50"/>
-      <c r="E116" s="110"/>
-      <c r="F116" s="110"/>
-      <c r="G116" s="110"/>
+      <c r="E116" s="109"/>
+      <c r="F116" s="109"/>
+      <c r="G116" s="109"/>
       <c r="H116" s="50"/>
       <c r="I116" s="50"/>
       <c r="J116" s="51"/>
@@ -3589,7 +3575,7 @@
       <c r="D118" s="10"/>
       <c r="E118" s="17"/>
       <c r="F118" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G118" s="45"/>
       <c r="H118" s="10"/>
@@ -3623,10 +3609,10 @@
       <c r="C121" s="52"/>
       <c r="D121" s="17"/>
       <c r="E121" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F121" s="57" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G121" s="17"/>
       <c r="H121" s="17"/>
@@ -3638,7 +3624,7 @@
       <c r="C122" s="52"/>
       <c r="D122" s="17"/>
       <c r="E122" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F122" s="56">
         <v>450</v>
@@ -3653,7 +3639,7 @@
       <c r="C123" s="52"/>
       <c r="D123" s="17"/>
       <c r="E123" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F123" s="58">
         <v>9</v>
@@ -3668,7 +3654,7 @@
       <c r="C124" s="52"/>
       <c r="D124" s="17"/>
       <c r="E124" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F124" s="17"/>
       <c r="G124" s="17"/>
@@ -3692,11 +3678,11 @@
       <c r="C126" s="52"/>
       <c r="D126" s="17"/>
       <c r="E126" s="60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F126" s="17"/>
       <c r="G126" s="61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H126" s="17"/>
       <c r="I126" s="52"/>
@@ -3726,34 +3712,34 @@
     </row>
     <row r="131" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B131" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="132" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B132" s="97" t="s">
+        <v>121</v>
+      </c>
+      <c r="C132" s="97"/>
+      <c r="D132" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E132" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F132" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="G132" s="30" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="132" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B132" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="C132" s="102"/>
-      <c r="D132" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E132" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F132" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="G132" s="30" t="s">
+      <c r="H132" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="H132" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="I132" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J132" s="32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="133" spans="2:10" x14ac:dyDescent="0.3">
@@ -3770,12 +3756,12 @@
     <row r="134" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B134" s="22"/>
       <c r="C134" s="34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D134" s="23"/>
-      <c r="E134" s="99"/>
-      <c r="F134" s="99"/>
-      <c r="G134" s="99"/>
+      <c r="E134" s="95"/>
+      <c r="F134" s="95"/>
+      <c r="G134" s="95"/>
       <c r="H134" s="23"/>
       <c r="I134" s="23"/>
       <c r="J134" s="24"/>
@@ -3795,9 +3781,9 @@
       <c r="B136" s="26"/>
       <c r="C136" s="10"/>
       <c r="D136" s="10"/>
-      <c r="E136" s="101"/>
-      <c r="F136" s="101"/>
-      <c r="G136" s="101"/>
+      <c r="E136" s="96"/>
+      <c r="F136" s="96"/>
+      <c r="G136" s="96"/>
       <c r="H136" s="10"/>
       <c r="I136" s="10"/>
       <c r="J136" s="27"/>
@@ -3806,9 +3792,9 @@
       <c r="B137" s="26"/>
       <c r="C137" s="10"/>
       <c r="D137" s="10"/>
-      <c r="E137" s="103"/>
-      <c r="F137" s="103"/>
-      <c r="G137" s="103"/>
+      <c r="E137" s="107"/>
+      <c r="F137" s="107"/>
+      <c r="G137" s="107"/>
       <c r="H137" s="10"/>
       <c r="I137" s="10"/>
       <c r="J137" s="27"/>
@@ -3816,7 +3802,7 @@
     <row r="138" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B138" s="26"/>
       <c r="C138" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D138" s="10"/>
       <c r="H138" s="17"/>
@@ -3826,16 +3812,16 @@
     <row r="139" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B139" s="26"/>
       <c r="C139" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D139" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E139" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="E139" s="42" t="s">
+      <c r="F139" s="42" t="s">
         <v>61</v>
-      </c>
-      <c r="F139" s="42" t="s">
-        <v>62</v>
       </c>
       <c r="G139" s="42"/>
       <c r="H139" s="14"/>
@@ -3845,7 +3831,7 @@
     <row r="140" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B140" s="26"/>
       <c r="C140" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D140" s="17">
         <v>4050</v>
@@ -3859,7 +3845,7 @@
       <c r="G140" s="17"/>
       <c r="H140" s="17"/>
       <c r="I140" s="59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J140" s="27"/>
     </row>
@@ -3963,30 +3949,30 @@
       <c r="J149" s="29"/>
     </row>
     <row r="151" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B151" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="C151" s="102"/>
+      <c r="B151" s="97" t="s">
+        <v>121</v>
+      </c>
+      <c r="C151" s="97"/>
       <c r="D151" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E151" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="F151" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F151" s="30" t="s">
+      <c r="G151" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="G151" s="30" t="s">
+      <c r="H151" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="H151" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="I151" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J151" s="32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="152" spans="2:10" x14ac:dyDescent="0.3">
@@ -4003,12 +3989,12 @@
     <row r="153" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B153" s="22"/>
       <c r="C153" s="34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D153" s="23"/>
-      <c r="E153" s="99"/>
-      <c r="F153" s="99"/>
-      <c r="G153" s="99"/>
+      <c r="E153" s="95"/>
+      <c r="F153" s="95"/>
+      <c r="G153" s="95"/>
       <c r="H153" s="23"/>
       <c r="I153" s="23"/>
       <c r="J153" s="24"/>
@@ -4028,9 +4014,9 @@
       <c r="B155" s="49"/>
       <c r="C155" s="50"/>
       <c r="D155" s="50"/>
-      <c r="E155" s="109"/>
-      <c r="F155" s="109"/>
-      <c r="G155" s="109"/>
+      <c r="E155" s="108"/>
+      <c r="F155" s="108"/>
+      <c r="G155" s="108"/>
       <c r="H155" s="50"/>
       <c r="I155" s="50"/>
       <c r="J155" s="51"/>
@@ -4039,9 +4025,9 @@
       <c r="B156" s="49"/>
       <c r="C156" s="50"/>
       <c r="D156" s="50"/>
-      <c r="E156" s="110"/>
-      <c r="F156" s="110"/>
-      <c r="G156" s="110"/>
+      <c r="E156" s="109"/>
+      <c r="F156" s="109"/>
+      <c r="G156" s="109"/>
       <c r="H156" s="50"/>
       <c r="I156" s="50"/>
       <c r="J156" s="51"/>
@@ -4092,10 +4078,10 @@
       <c r="C161" s="52"/>
       <c r="D161" s="17"/>
       <c r="E161" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F161" s="57" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G161" s="17"/>
       <c r="H161" s="17"/>
@@ -4107,7 +4093,7 @@
       <c r="C162" s="52"/>
       <c r="D162" s="17"/>
       <c r="E162" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F162" s="56">
         <v>450</v>
@@ -4122,13 +4108,13 @@
       <c r="C163" s="52"/>
       <c r="D163" s="17"/>
       <c r="E163" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F163" s="58">
         <v>9</v>
       </c>
       <c r="G163" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H163" s="17"/>
       <c r="I163" s="52"/>
@@ -4161,11 +4147,11 @@
       <c r="C166" s="52"/>
       <c r="D166" s="17"/>
       <c r="E166" s="60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F166" s="17"/>
       <c r="G166" s="63" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H166" s="17"/>
       <c r="I166" s="52"/>
@@ -4195,34 +4181,34 @@
     </row>
     <row r="172" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B172" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="173" spans="2:27" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B173" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="C173" s="102"/>
+      <c r="B173" s="97" t="s">
+        <v>121</v>
+      </c>
+      <c r="C173" s="97"/>
       <c r="D173" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E173" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F173" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F173" s="30" t="s">
+      <c r="G173" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="G173" s="44" t="s">
+      <c r="H173" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="H173" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="I173" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J173" s="32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="174" spans="2:27" x14ac:dyDescent="0.3">
@@ -4239,12 +4225,12 @@
     <row r="175" spans="2:27" ht="18" x14ac:dyDescent="0.35">
       <c r="B175" s="22"/>
       <c r="C175" s="34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D175" s="23"/>
-      <c r="E175" s="99"/>
-      <c r="F175" s="99"/>
-      <c r="G175" s="99"/>
+      <c r="E175" s="95"/>
+      <c r="F175" s="95"/>
+      <c r="G175" s="95"/>
       <c r="H175" s="23"/>
       <c r="I175" s="23"/>
       <c r="J175" s="24"/>
@@ -4312,11 +4298,11 @@
       <c r="B177" s="26"/>
       <c r="C177" s="10"/>
       <c r="D177" s="10"/>
-      <c r="E177" s="101"/>
-      <c r="F177" s="101"/>
-      <c r="G177" s="101"/>
+      <c r="E177" s="96"/>
+      <c r="F177" s="96"/>
+      <c r="G177" s="96"/>
       <c r="H177" s="71" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I177" s="10"/>
       <c r="J177" s="27"/>
@@ -4325,14 +4311,14 @@
       <c r="B178" s="26"/>
       <c r="C178" s="10"/>
       <c r="D178" s="10"/>
-      <c r="E178" s="103" t="s">
-        <v>66</v>
-      </c>
-      <c r="F178" s="103"/>
-      <c r="G178" s="103"/>
+      <c r="E178" s="107" t="s">
+        <v>65</v>
+      </c>
+      <c r="F178" s="107"/>
+      <c r="G178" s="107"/>
       <c r="H178" s="10"/>
       <c r="I178" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J178" s="27"/>
     </row>
@@ -4439,19 +4425,19 @@
       <c r="B188" s="26"/>
       <c r="C188" s="17"/>
       <c r="D188" s="72" t="s">
+        <v>70</v>
+      </c>
+      <c r="E188" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="E188" s="72" t="s">
+      <c r="F188" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="F188" s="72" t="s">
+      <c r="G188" s="72" t="s">
+        <v>74</v>
+      </c>
+      <c r="H188" s="73" t="s">
         <v>73</v>
-      </c>
-      <c r="G188" s="72" t="s">
-        <v>75</v>
-      </c>
-      <c r="H188" s="73" t="s">
-        <v>74</v>
       </c>
       <c r="I188" s="17"/>
       <c r="J188" s="27"/>
@@ -4459,7 +4445,7 @@
     <row r="189" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B189" s="26"/>
       <c r="C189" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D189" s="17"/>
       <c r="E189" s="17"/>
@@ -4483,17 +4469,17 @@
     <row r="191" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B191" s="26"/>
       <c r="C191" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D191" s="10"/>
       <c r="E191" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F191" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G191" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="F191" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G191" s="10" t="s">
-        <v>70</v>
       </c>
       <c r="H191" s="10"/>
       <c r="I191" s="10"/>
@@ -4502,7 +4488,7 @@
     <row r="192" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B192" s="26"/>
       <c r="C192" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D192" s="10"/>
       <c r="E192" s="69">
@@ -4521,7 +4507,7 @@
     <row r="193" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B193" s="26"/>
       <c r="C193" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D193" s="10"/>
       <c r="E193" s="69">
@@ -4531,7 +4517,7 @@
         <v>30</v>
       </c>
       <c r="G193" s="57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H193" s="10"/>
       <c r="I193" s="10"/>
@@ -4573,7 +4559,7 @@
     <row r="197" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B197" s="26"/>
       <c r="C197" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D197" s="10"/>
       <c r="E197" s="10"/>
@@ -4581,17 +4567,17 @@
       <c r="G197" s="10"/>
       <c r="H197" s="10"/>
       <c r="I197" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J197" s="27"/>
     </row>
     <row r="198" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B198" s="26"/>
       <c r="C198" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D198" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="D198" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="E198" s="10"/>
       <c r="F198" s="10"/>
@@ -4625,7 +4611,7 @@
     <row r="201" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B201" s="26"/>
       <c r="C201" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D201" s="10"/>
       <c r="E201" s="10"/>
@@ -4633,17 +4619,17 @@
       <c r="G201" s="10"/>
       <c r="H201" s="10"/>
       <c r="I201" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J201" s="27"/>
     </row>
     <row r="202" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B202" s="26"/>
       <c r="C202" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D202" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E202" s="10"/>
       <c r="F202" s="10"/>
@@ -4698,34 +4684,34 @@
     </row>
     <row r="209" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B209" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="210" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B210" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="C210" s="102"/>
+      <c r="B210" s="97" t="s">
+        <v>121</v>
+      </c>
+      <c r="C210" s="97"/>
       <c r="D210" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E210" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F210" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F210" s="30" t="s">
+      <c r="G210" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="G210" s="30" t="s">
+      <c r="H210" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="H210" s="33" t="s">
-        <v>18</v>
-      </c>
       <c r="I210" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J210" s="32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="211" spans="2:10" x14ac:dyDescent="0.3">
@@ -4742,12 +4728,12 @@
     <row r="212" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B212" s="22"/>
       <c r="C212" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D212" s="23"/>
-      <c r="E212" s="99"/>
-      <c r="F212" s="99"/>
-      <c r="G212" s="99"/>
+      <c r="E212" s="95"/>
+      <c r="F212" s="95"/>
+      <c r="G212" s="95"/>
       <c r="H212" s="23"/>
       <c r="I212" s="23"/>
       <c r="J212" s="24"/>
@@ -4767,9 +4753,9 @@
       <c r="B214" s="26"/>
       <c r="C214" s="10"/>
       <c r="D214" s="10"/>
-      <c r="E214" s="101"/>
-      <c r="F214" s="101"/>
-      <c r="G214" s="101"/>
+      <c r="E214" s="96"/>
+      <c r="F214" s="96"/>
+      <c r="G214" s="96"/>
       <c r="H214" s="10"/>
       <c r="I214" s="10"/>
       <c r="J214" s="27"/>
@@ -4777,19 +4763,19 @@
     <row r="215" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B215" s="26"/>
       <c r="D215" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E215" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F215" s="80" t="s">
+        <v>59</v>
+      </c>
+      <c r="G215" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="F215" s="80" t="s">
-        <v>60</v>
-      </c>
-      <c r="G215" s="80" t="s">
+      <c r="H215" s="80" t="s">
         <v>88</v>
-      </c>
-      <c r="H215" s="80" t="s">
-        <v>89</v>
       </c>
       <c r="I215" s="10"/>
       <c r="J215" s="27"/>
@@ -4797,10 +4783,10 @@
     <row r="216" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B216" s="26"/>
       <c r="D216" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E216" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F216" s="76">
         <v>432</v>
@@ -4822,10 +4808,10 @@
     <row r="218" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B218" s="26"/>
       <c r="D218" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E218" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F218" s="56">
         <v>4000</v>
@@ -4854,10 +4840,10 @@
       <c r="B220" s="26"/>
       <c r="C220" s="17"/>
       <c r="D220" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E220" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F220" s="56">
         <v>50</v>
@@ -4950,34 +4936,34 @@
     </row>
     <row r="229" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B229" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="230" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B230" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="C230" s="102"/>
+      <c r="B230" s="97" t="s">
+        <v>121</v>
+      </c>
+      <c r="C230" s="97"/>
       <c r="D230" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E230" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F230" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F230" s="30" t="s">
+      <c r="G230" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="G230" s="30" t="s">
+      <c r="H230" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="H230" s="31" t="s">
-        <v>18</v>
-      </c>
       <c r="I230" s="33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J230" s="32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="231" spans="2:10" x14ac:dyDescent="0.3">
@@ -4995,9 +4981,9 @@
       <c r="B232" s="22"/>
       <c r="C232" s="34"/>
       <c r="D232" s="23"/>
-      <c r="E232" s="99"/>
-      <c r="F232" s="99"/>
-      <c r="G232" s="99"/>
+      <c r="E232" s="95"/>
+      <c r="F232" s="95"/>
+      <c r="G232" s="95"/>
       <c r="H232" s="23"/>
       <c r="I232" s="23"/>
       <c r="J232" s="24"/>
@@ -5005,7 +4991,7 @@
     <row r="233" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B233" s="22"/>
       <c r="C233" s="83" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D233" s="23"/>
       <c r="E233" s="23"/>
@@ -5019,9 +5005,9 @@
       <c r="B234" s="22"/>
       <c r="C234" s="23"/>
       <c r="D234" s="23"/>
-      <c r="E234" s="100"/>
-      <c r="F234" s="100"/>
-      <c r="G234" s="100"/>
+      <c r="E234" s="112"/>
+      <c r="F234" s="112"/>
+      <c r="G234" s="112"/>
       <c r="H234" s="23"/>
       <c r="I234" s="23"/>
       <c r="J234" s="24"/>
@@ -5054,7 +5040,7 @@
       <c r="D237" s="10"/>
       <c r="E237" s="10"/>
       <c r="F237" s="85" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G237" s="10"/>
       <c r="H237" s="10"/>
@@ -5075,14 +5061,14 @@
       <c r="B239" s="26"/>
       <c r="C239" s="17"/>
       <c r="D239" s="17"/>
-      <c r="E239" s="101" t="s">
-        <v>101</v>
-      </c>
-      <c r="F239" s="101"/>
-      <c r="G239" s="101"/>
+      <c r="E239" s="96" t="s">
+        <v>100</v>
+      </c>
+      <c r="F239" s="96"/>
+      <c r="G239" s="96"/>
       <c r="H239" s="17"/>
       <c r="I239" s="47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J239" s="27"/>
     </row>
@@ -5101,11 +5087,11 @@
       <c r="B241" s="26"/>
       <c r="C241" s="17"/>
       <c r="D241" s="17"/>
-      <c r="E241" s="97" t="s">
-        <v>102</v>
-      </c>
-      <c r="F241" s="97"/>
-      <c r="G241" s="97"/>
+      <c r="E241" s="104" t="s">
+        <v>101</v>
+      </c>
+      <c r="F241" s="104"/>
+      <c r="G241" s="104"/>
       <c r="H241" s="17"/>
       <c r="I241" s="17"/>
       <c r="J241" s="27"/>
@@ -5114,11 +5100,11 @@
       <c r="B242" s="26"/>
       <c r="C242" s="17"/>
       <c r="D242" s="17"/>
-      <c r="E242" s="96">
+      <c r="E242" s="110">
         <v>6000</v>
       </c>
-      <c r="F242" s="97"/>
-      <c r="G242" s="97"/>
+      <c r="F242" s="104"/>
+      <c r="G242" s="104"/>
       <c r="H242" s="17"/>
       <c r="I242" s="17"/>
       <c r="J242" s="27"/>
@@ -5138,11 +5124,11 @@
       <c r="B244" s="26"/>
       <c r="C244" s="17"/>
       <c r="D244" s="17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E244" s="17"/>
       <c r="F244" s="46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G244" s="17"/>
       <c r="H244" s="17"/>
@@ -5153,11 +5139,11 @@
       <c r="B245" s="26"/>
       <c r="C245" s="17"/>
       <c r="D245" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E245" s="17"/>
       <c r="F245" s="46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G245" s="17"/>
       <c r="H245" s="17"/>
@@ -5168,16 +5154,16 @@
       <c r="B246" s="26"/>
       <c r="C246" s="17"/>
       <c r="D246" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E246" s="17"/>
       <c r="F246" s="89" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G246" s="17"/>
       <c r="H246" s="17"/>
       <c r="I246" s="47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J246" s="27"/>
     </row>
@@ -5185,7 +5171,7 @@
       <c r="B247" s="26"/>
       <c r="C247" s="10"/>
       <c r="D247" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E247" s="10"/>
       <c r="F247" s="90">
@@ -5211,11 +5197,11 @@
       <c r="B249" s="26"/>
       <c r="C249" s="10"/>
       <c r="D249" s="10"/>
-      <c r="E249" s="98" t="s">
-        <v>106</v>
-      </c>
-      <c r="F249" s="98"/>
-      <c r="G249" s="98"/>
+      <c r="E249" s="111" t="s">
+        <v>105</v>
+      </c>
+      <c r="F249" s="111"/>
+      <c r="G249" s="111"/>
       <c r="H249" s="10"/>
       <c r="I249" s="10"/>
       <c r="J249" s="27"/>
@@ -5244,10 +5230,10 @@
     </row>
     <row r="255" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B255" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="257" spans="2:9" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="257" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C257" s="74"/>
       <c r="D257" s="6"/>
       <c r="E257" s="6"/>
@@ -5256,10 +5242,10 @@
       <c r="H257" s="6"/>
       <c r="I257" s="75"/>
     </row>
-    <row r="258" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="258" spans="3:9" ht="18" x14ac:dyDescent="0.35">
       <c r="C258" s="26"/>
       <c r="D258" s="84" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E258" s="10"/>
       <c r="F258" s="10"/>
@@ -5267,7 +5253,7 @@
       <c r="H258" s="10"/>
       <c r="I258" s="27"/>
     </row>
-    <row r="259" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="259" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C259" s="26"/>
       <c r="D259" s="10"/>
       <c r="E259" s="10"/>
@@ -5276,20 +5262,20 @@
       <c r="H259" s="10"/>
       <c r="I259" s="27"/>
     </row>
-    <row r="260" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="260" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C260" s="26"/>
       <c r="D260" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E260" s="10"/>
       <c r="F260" s="10"/>
       <c r="G260" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H260" s="3"/>
       <c r="I260" s="27"/>
     </row>
-    <row r="261" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="261" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C261" s="26"/>
       <c r="D261" s="10"/>
       <c r="E261" s="10"/>
@@ -5298,20 +5284,20 @@
       <c r="H261" s="10"/>
       <c r="I261" s="27"/>
     </row>
-    <row r="262" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="262" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C262" s="26"/>
       <c r="D262" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E262" s="10"/>
       <c r="F262" s="10"/>
       <c r="G262" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H262" s="3"/>
       <c r="I262" s="27"/>
     </row>
-    <row r="263" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="263" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C263" s="26"/>
       <c r="D263" s="10"/>
       <c r="E263" s="10"/>
@@ -5320,7 +5306,7 @@
       <c r="H263" s="10"/>
       <c r="I263" s="27"/>
     </row>
-    <row r="264" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="264" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C264" s="26"/>
       <c r="D264" s="10"/>
       <c r="E264" s="10"/>
@@ -5329,20 +5315,20 @@
       <c r="H264" s="10"/>
       <c r="I264" s="27"/>
     </row>
-    <row r="265" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="265" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C265" s="26"/>
       <c r="D265" s="10"/>
-      <c r="E265" s="23" t="s">
-        <v>57</v>
+      <c r="E265" s="94" t="s">
+        <v>56</v>
       </c>
       <c r="F265" s="10"/>
-      <c r="G265" s="23" t="s">
-        <v>111</v>
+      <c r="G265" s="94" t="s">
+        <v>110</v>
       </c>
       <c r="H265" s="10"/>
       <c r="I265" s="27"/>
     </row>
-    <row r="266" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="266" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C266" s="28"/>
       <c r="D266" s="14"/>
       <c r="E266" s="14"/>
@@ -5351,94 +5337,51 @@
       <c r="H266" s="14"/>
       <c r="I266" s="29"/>
     </row>
-    <row r="270" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B270" s="1" t="s">
+    <row r="273" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B273" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="272" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C272" s="74"/>
-      <c r="D272" s="6"/>
-      <c r="E272" s="6"/>
-      <c r="F272" s="6"/>
-      <c r="G272" s="6"/>
-      <c r="H272" s="6"/>
-      <c r="I272" s="75"/>
-    </row>
-    <row r="273" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="C273" s="26"/>
-      <c r="D273" s="84" t="s">
+    <row r="275" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C275" s="74"/>
+      <c r="D275" s="6"/>
+      <c r="E275" s="6"/>
+      <c r="F275" s="6"/>
+      <c r="G275" s="6"/>
+      <c r="H275" s="6"/>
+      <c r="I275" s="75"/>
+    </row>
+    <row r="276" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="C276" s="26"/>
+      <c r="D276" s="84" t="s">
         <v>115</v>
       </c>
-      <c r="E273" s="10"/>
-      <c r="F273" s="10"/>
-      <c r="G273" s="10"/>
-      <c r="H273" s="10"/>
-      <c r="I273" s="27"/>
-    </row>
-    <row r="274" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C274" s="26"/>
-      <c r="D274" s="10"/>
-      <c r="E274" s="10"/>
-      <c r="F274" s="10"/>
-      <c r="G274" s="10"/>
-      <c r="H274" s="10"/>
-      <c r="I274" s="27"/>
-    </row>
-    <row r="275" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C275" s="26"/>
-      <c r="D275" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E275" s="10"/>
-      <c r="F275" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="G275" s="10"/>
-      <c r="H275" s="10"/>
-      <c r="I275" s="27"/>
-    </row>
-    <row r="276" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C276" s="26"/>
-      <c r="D276" s="10"/>
       <c r="E276" s="10"/>
       <c r="F276" s="10"/>
       <c r="G276" s="10"/>
       <c r="H276" s="10"/>
       <c r="I276" s="27"/>
     </row>
-    <row r="277" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C277" s="26"/>
-      <c r="D277" s="10" t="s">
-        <v>118</v>
-      </c>
+      <c r="D277" s="10"/>
       <c r="E277" s="10"/>
-      <c r="F277" s="86" t="s">
-        <v>97</v>
-      </c>
-      <c r="G277" s="91" t="s">
-        <v>98</v>
-      </c>
-      <c r="H277" s="92" t="s">
-        <v>99</v>
-      </c>
+      <c r="F277" s="10"/>
+      <c r="G277" s="10"/>
+      <c r="H277" s="10"/>
       <c r="I277" s="27"/>
     </row>
     <row r="278" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C278" s="26"/>
       <c r="D278" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E278" s="10"/>
-      <c r="F278" s="69">
-        <v>2500</v>
-      </c>
-      <c r="G278" s="69">
-        <v>5000</v>
-      </c>
-      <c r="H278" s="69">
-        <v>10000</v>
-      </c>
+      <c r="F278" s="91" t="s">
+        <v>104</v>
+      </c>
+      <c r="G278" s="10"/>
+      <c r="H278" s="10"/>
       <c r="I278" s="27"/>
     </row>
     <row r="279" spans="2:9" x14ac:dyDescent="0.3">
@@ -5452,137 +5395,104 @@
     </row>
     <row r="280" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C280" s="26"/>
-      <c r="D280" s="10"/>
-      <c r="E280" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="F280" s="10"/>
-      <c r="G280" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="H280" s="10"/>
+      <c r="D280" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E280" s="10"/>
+      <c r="F280" s="93" t="s">
+        <v>117</v>
+      </c>
+      <c r="G280" s="92"/>
+      <c r="H280" s="3"/>
       <c r="I280" s="27"/>
     </row>
     <row r="281" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C281" s="28"/>
-      <c r="D281" s="14"/>
-      <c r="E281" s="14"/>
-      <c r="F281" s="14"/>
-      <c r="G281" s="14"/>
-      <c r="H281" s="14"/>
-      <c r="I281" s="29"/>
-    </row>
-    <row r="285" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B285" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="287" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C287" s="74"/>
-      <c r="D287" s="6"/>
-      <c r="E287" s="6"/>
-      <c r="F287" s="6"/>
-      <c r="G287" s="6"/>
-      <c r="H287" s="6"/>
-      <c r="I287" s="75"/>
-    </row>
-    <row r="288" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="C288" s="26"/>
-      <c r="D288" s="84" t="s">
-        <v>121</v>
-      </c>
-      <c r="E288" s="10"/>
-      <c r="F288" s="10"/>
-      <c r="G288" s="10"/>
-      <c r="H288" s="10"/>
-      <c r="I288" s="27"/>
-    </row>
-    <row r="289" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C289" s="26"/>
-      <c r="D289" s="10"/>
-      <c r="E289" s="10"/>
-      <c r="F289" s="10"/>
-      <c r="G289" s="10"/>
-      <c r="H289" s="10"/>
-      <c r="I289" s="27"/>
-    </row>
-    <row r="290" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C290" s="26"/>
-      <c r="D290" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="E290" s="10"/>
-      <c r="F290" s="93" t="s">
-        <v>105</v>
-      </c>
-      <c r="G290" s="10"/>
-      <c r="H290" s="10"/>
-      <c r="I290" s="27"/>
-    </row>
-    <row r="291" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C291" s="26"/>
-      <c r="D291" s="10"/>
-      <c r="E291" s="10"/>
-      <c r="F291" s="10"/>
-      <c r="G291" s="10"/>
-      <c r="H291" s="10"/>
-      <c r="I291" s="27"/>
-    </row>
-    <row r="292" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C292" s="26"/>
-      <c r="D292" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="E292" s="10"/>
-      <c r="F292" s="95" t="s">
-        <v>123</v>
-      </c>
-      <c r="G292" s="94"/>
-      <c r="H292" s="3"/>
-      <c r="I292" s="27"/>
-    </row>
-    <row r="293" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C293" s="26"/>
-      <c r="D293" s="10"/>
-      <c r="E293" s="10"/>
-      <c r="F293" s="69"/>
-      <c r="G293" s="69"/>
-      <c r="H293" s="69"/>
-      <c r="I293" s="27"/>
-    </row>
-    <row r="294" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C294" s="26"/>
-      <c r="D294" s="10"/>
-      <c r="E294" s="10"/>
-      <c r="F294" s="10"/>
-      <c r="G294" s="10"/>
-      <c r="H294" s="10"/>
-      <c r="I294" s="27"/>
-    </row>
-    <row r="295" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C295" s="26"/>
-      <c r="D295" s="10"/>
-      <c r="E295" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="F295" s="10"/>
-      <c r="G295" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="H295" s="10"/>
-      <c r="I295" s="27"/>
-    </row>
-    <row r="296" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C296" s="28"/>
-      <c r="D296" s="14"/>
-      <c r="E296" s="14"/>
-      <c r="F296" s="14"/>
-      <c r="G296" s="14"/>
-      <c r="H296" s="14"/>
-      <c r="I296" s="29"/>
+      <c r="C281" s="26"/>
+      <c r="D281" s="10"/>
+      <c r="E281" s="10"/>
+      <c r="F281" s="69"/>
+      <c r="G281" s="69"/>
+      <c r="H281" s="69"/>
+      <c r="I281" s="27"/>
+    </row>
+    <row r="282" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C282" s="26"/>
+      <c r="D282" s="10"/>
+      <c r="E282" s="10"/>
+      <c r="F282" s="10"/>
+      <c r="G282" s="10"/>
+      <c r="H282" s="10"/>
+      <c r="I282" s="27"/>
+    </row>
+    <row r="283" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C283" s="26"/>
+      <c r="D283" s="10"/>
+      <c r="E283" s="94" t="s">
+        <v>56</v>
+      </c>
+      <c r="F283" s="10"/>
+      <c r="G283" s="94" t="s">
+        <v>110</v>
+      </c>
+      <c r="H283" s="10"/>
+      <c r="I283" s="27"/>
+    </row>
+    <row r="284" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C284" s="28"/>
+      <c r="D284" s="14"/>
+      <c r="E284" s="14"/>
+      <c r="F284" s="14"/>
+      <c r="G284" s="14"/>
+      <c r="H284" s="14"/>
+      <c r="I284" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="E242:G242"/>
+    <mergeCell ref="E249:G249"/>
+    <mergeCell ref="E232:G232"/>
+    <mergeCell ref="E234:G234"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E239:G239"/>
+    <mergeCell ref="E241:G241"/>
+    <mergeCell ref="E96:G96"/>
+    <mergeCell ref="C57:I57"/>
+    <mergeCell ref="C58:I58"/>
+    <mergeCell ref="C59:I59"/>
+    <mergeCell ref="C55:I55"/>
+    <mergeCell ref="C56:I56"/>
+    <mergeCell ref="E155:G155"/>
+    <mergeCell ref="E156:G156"/>
+    <mergeCell ref="B173:C173"/>
+    <mergeCell ref="B210:C210"/>
+    <mergeCell ref="E212:G212"/>
+    <mergeCell ref="E214:G214"/>
+    <mergeCell ref="B230:C230"/>
+    <mergeCell ref="E97:G97"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="E113:G113"/>
+    <mergeCell ref="E115:G115"/>
+    <mergeCell ref="E116:G116"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="E134:G134"/>
+    <mergeCell ref="E136:G136"/>
+    <mergeCell ref="E137:G137"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="E153:G153"/>
+    <mergeCell ref="E178:G178"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="E94:G94"/>
+    <mergeCell ref="C60:I60"/>
+    <mergeCell ref="C61:I61"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E49:G49"/>
     <mergeCell ref="E175:G175"/>
     <mergeCell ref="E177:G177"/>
     <mergeCell ref="M3:N3"/>
@@ -5599,56 +5509,11 @@
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="E94:G94"/>
-    <mergeCell ref="C60:I60"/>
-    <mergeCell ref="C61:I61"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="B210:C210"/>
-    <mergeCell ref="E212:G212"/>
-    <mergeCell ref="E214:G214"/>
-    <mergeCell ref="B230:C230"/>
-    <mergeCell ref="E97:G97"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="E113:G113"/>
-    <mergeCell ref="E115:G115"/>
-    <mergeCell ref="E116:G116"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="E134:G134"/>
-    <mergeCell ref="E136:G136"/>
-    <mergeCell ref="E137:G137"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="E153:G153"/>
-    <mergeCell ref="E178:G178"/>
-    <mergeCell ref="E242:G242"/>
-    <mergeCell ref="E249:G249"/>
-    <mergeCell ref="E232:G232"/>
-    <mergeCell ref="E234:G234"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E239:G239"/>
-    <mergeCell ref="E241:G241"/>
-    <mergeCell ref="E96:G96"/>
-    <mergeCell ref="C57:I57"/>
-    <mergeCell ref="C58:I58"/>
-    <mergeCell ref="C59:I59"/>
-    <mergeCell ref="C55:I55"/>
-    <mergeCell ref="C56:I56"/>
-    <mergeCell ref="E155:G155"/>
-    <mergeCell ref="E156:G156"/>
-    <mergeCell ref="B173:C173"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F246" r:id="rId1" xr:uid="{6319A271-FBAA-4ADE-BE1A-6D52EFCC9A45}"/>
-    <hyperlink ref="F290" r:id="rId2" xr:uid="{845BDB71-FAB5-42EC-831B-42D96171F472}"/>
-    <hyperlink ref="F292" r:id="rId3" xr:uid="{2BB362DF-F303-43AC-BB03-CA234A5D662D}"/>
+    <hyperlink ref="F278" r:id="rId2" xr:uid="{845BDB71-FAB5-42EC-831B-42D96171F472}"/>
+    <hyperlink ref="F280" r:id="rId3" xr:uid="{2BB362DF-F303-43AC-BB03-CA234A5D662D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>

</xml_diff>